<commit_message>
update acm raw data
</commit_message>
<xml_diff>
--- a/02 screening results.xlsx
+++ b/02 screening results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\Repos\mde4dts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B87864-F6D1-4350-A43D-D8F255698C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898D8FAD-AC74-40FE-99E8-3DCB36C666CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exclusion Results" sheetId="2" r:id="rId1"/>
@@ -3360,8 +3360,8 @@
   </sheetPr>
   <dimension ref="A1:K924"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:G191"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B182" sqref="B182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -13806,8 +13806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC333BD6-FE25-4D66-90C9-A3143490C461}">
   <dimension ref="A1:H923"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
-      <selection activeCell="B186" sqref="B186"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>

</xml_diff>